<commit_message>
hausman and lmtests tables
</commit_message>
<xml_diff>
--- a/results/tables/spatial_hausman.xlsx
+++ b/results/tables/spatial_hausman.xlsx
@@ -377,12 +377,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ols</t>
+          <t>OLS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -394,12 +394,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sar</t>
+          <t>SAR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -411,12 +411,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>sem</t>
+          <t>SEM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -428,12 +428,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>sarar</t>
+          <t>SARAR</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -445,12 +445,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>sdm</t>
+          <t>SDM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -462,12 +462,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>sdem</t>
+          <t>SDEM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -479,12 +479,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>farsnocc</t>
+          <t>Log(TFVN)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>slx</t>
+          <t>SLX</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -496,12 +496,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ols</t>
+          <t>OLS</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -513,12 +513,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>sar</t>
+          <t>SAR</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -530,12 +530,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>sem</t>
+          <t>SEM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -547,12 +547,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>sarar</t>
+          <t>SARAR</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -564,24 +564,24 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>sdm</t>
+          <t>SDM</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>sdem</t>
+          <t>SDEM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -593,12 +593,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>farsocc</t>
+          <t>Log(TFVO)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>slx</t>
+          <t>SLX</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">

</xml_diff>